<commit_message>
Add missingness checks and correct missing date errors
</commit_message>
<xml_diff>
--- a/inst/extdata/drug_dict.xlsx
+++ b/inst/extdata/drug_dict.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -786,22 +786,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.58203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -824,7 +824,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>98</v>
       </c>
@@ -849,7 +849,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>99</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -920,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>91</v>
       </c>
@@ -966,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>93</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>43</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>51</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>61</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>78</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>62</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>79</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>80</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>63</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>81</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>64</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>65</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>66</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>67</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>68</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>82</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>83</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>97</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>95</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>84</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>85</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>86</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>87</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>69</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>3</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>4</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>96</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>100</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>101</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>102</v>
       </c>
@@ -2024,22 +2024,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F59" s="1"/>
     </row>
   </sheetData>

</xml_diff>